<commit_message>
Big update for new student year
</commit_message>
<xml_diff>
--- a/_site/script/alumni_info.xlsx
+++ b/_site/script/alumni_info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rl-lab\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rl.beiyang.ren\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6204D4B8-BB9F-421E-9DEE-8BF2837B35B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="129">
   <si>
     <t>序号</t>
   </si>
@@ -361,20 +362,98 @@
   </si>
   <si>
     <t>China Academy of Aerospace Scientce and Innovation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>吴吉洲</t>
+  </si>
+  <si>
+    <t>Jizhou Wu</t>
+  </si>
+  <si>
+    <t>Deep Reinforcement Learning, Transfer learning</t>
+  </si>
+  <si>
+    <t>https://github.com/Cubism-star</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_13_q7_1691548718NKzDT4.jpg?attname=13_7_%e9%9b%aa.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:jVJFkHHXDuk4weOKt5hUdbavARs=</t>
+  </si>
+  <si>
+    <t>胡肖汉</t>
+  </si>
+  <si>
+    <t>Xiaohan Hu</t>
+  </si>
+  <si>
+    <t>Offline reinforcement learning</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_14_q7_1691549520yan4kr.jpg?attname=15_7_gu.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:s4l0za4jwk_8A33HjHeXvM5avg0=</t>
+  </si>
+  <si>
+    <t>赵楷</t>
+  </si>
+  <si>
+    <t>Kai Zhao</t>
+  </si>
+  <si>
+    <t>Offline Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_15_q7_16915498024if4ae.jpg?attname=16_7_1%e5%af%b8%e7%85%a7-%e8%b5%b5%e6%a5%b7-%e7%99%bd%e5%ba%951-1.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:RleMeKmDk6KTi7qwpBdCD8NDGio=</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bilibili</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>孙琦淞</t>
+  </si>
+  <si>
+    <t>Qisong Sun</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning, Automated Negotiation</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_24_q7_1691997701MFS5J4.jpg?attname=24_7_%e8%af%81%e4%bb%b6%e7%85%a7.jpg&amp;e=1699841047&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:thoLcO0bQyZ0s7K0SQLD-pB7kz4=</t>
+  </si>
+  <si>
+    <t>杨阳</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang Yang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deep Reinforcement Learning, Artificial Intelligence</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_21_q7_1691576043idtDEj.jpg?attname=21_7_IMG_20230809_181326.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:P9SVD4R9x7HwpV5Q8WC4e7EpC5I=</t>
+  </si>
+  <si>
+    <t>Li Auto Inc.</t>
+  </si>
+  <si>
+    <t>Li Auto Inc.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -397,6 +476,19 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF040C28"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -415,7 +507,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -423,19 +515,23 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Comma" xfId="4"/>
-    <cellStyle name="Comma [0]" xfId="5"/>
-    <cellStyle name="Currency" xfId="2"/>
-    <cellStyle name="Currency [0]" xfId="3"/>
-    <cellStyle name="Normal" xfId="6"/>
-    <cellStyle name="Percent" xfId="1"/>
+  <cellStyles count="8">
+    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -769,11 +865,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -823,301 +919,298 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="D2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E3">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>12</v>
+      <c r="I3" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="D4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E4">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
-        <v>87</v>
-      </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="D5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
+        <v>118</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
+        <v>2021</v>
+      </c>
+      <c r="E6">
+        <v>2024</v>
+      </c>
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>2019</v>
-      </c>
-      <c r="E6">
-        <v>2022</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J6" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="E7">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="E8">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>2020</v>
+      </c>
+      <c r="E9">
+        <v>2023</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <v>2019</v>
-      </c>
-      <c r="E9">
-        <v>2022</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
       <c r="H9" t="s">
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="E10">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>2019</v>
@@ -1129,27 +1222,27 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>2019</v>
@@ -1161,27 +1254,27 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="J12" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D13">
         <v>2019</v>
@@ -1193,187 +1286,187 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D14">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E14">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H14" t="s">
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D15">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E15">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="D16">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E16">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D17">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E17">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H17" t="s">
         <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D18">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E18">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="D19">
         <v>2018</v>
@@ -1385,56 +1478,219 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="H19" t="s">
         <v>4</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J19" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>2018</v>
+      </c>
+      <c r="E20">
+        <v>2021</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>2018</v>
+      </c>
+      <c r="E21">
+        <v>2021</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22">
+        <v>2018</v>
+      </c>
+      <c r="E22">
+        <v>2021</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23">
+        <v>2018</v>
+      </c>
+      <c r="E23">
+        <v>2021</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24">
+        <v>2018</v>
+      </c>
+      <c r="E24">
+        <v>2021</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>12</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C25" t="s">
         <v>32</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>2017</v>
       </c>
-      <c r="E20">
+      <c r="E25">
         <v>2020</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
         <v>33</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H25" t="s">
         <v>34</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I25" t="s">
         <v>85</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J25" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J29">
     <sortCondition descending="1" ref="E1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{C5DFC761-3923-4EB6-ADCC-022C9BBE6EA0}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>